<commit_message>
ehh its good but not that good
</commit_message>
<xml_diff>
--- a/dump/Students.xlsx
+++ b/dump/Students.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BahaypareNHS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\BahaypareNHS\dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="189">
   <si>
     <t>Building 1</t>
   </si>
@@ -237,6 +237,360 @@
   </si>
   <si>
     <t>ARGANA, ERICKA, MANLIWAT.</t>
+  </si>
+  <si>
+    <t>Grade7</t>
+  </si>
+  <si>
+    <t>VIETNAM</t>
+  </si>
+  <si>
+    <t>ABLAZA, PRINCESS EIFFER DIZON</t>
+  </si>
+  <si>
+    <t>ALVAREZ, JOSELITO TOLENTINO JR.</t>
+  </si>
+  <si>
+    <t>AGUINALDO, ANGIE BUTIAL</t>
+  </si>
+  <si>
+    <t>BALUYOT, JAMES JAYSTER GALVAN</t>
+  </si>
+  <si>
+    <t>BUCANI, MARICEL HERNANDEZ</t>
+  </si>
+  <si>
+    <t>THAILAND</t>
+  </si>
+  <si>
+    <t>MALAYSIA</t>
+  </si>
+  <si>
+    <t>PHILIPPINES</t>
+  </si>
+  <si>
+    <t>Acuña, Megan Dela Mines</t>
+  </si>
+  <si>
+    <t>Aquino, Dylan</t>
+  </si>
+  <si>
+    <t>Aquino, Cloreed Puno</t>
+  </si>
+  <si>
+    <t>Baltazar, Warren De Guzman</t>
+  </si>
+  <si>
+    <t>Briones, Althea Nicole Tolentino</t>
+  </si>
+  <si>
+    <t>Bergado, James Carpio</t>
+  </si>
+  <si>
+    <t>Aquino, Michaela</t>
+  </si>
+  <si>
+    <t>Blas, Reniel Jassam Caones</t>
+  </si>
+  <si>
+    <t>Balajadia, Alica Zamantha Simbulan</t>
+  </si>
+  <si>
+    <t>Balajadia, Avygail Briz</t>
+  </si>
+  <si>
+    <t>AQUINO, YHANNEL ESCABAS</t>
+  </si>
+  <si>
+    <t>ALIGORA, RHYZZ LAUREEN FRANCISCO</t>
+  </si>
+  <si>
+    <t>CALMA, EURI SKY BULANADI</t>
+  </si>
+  <si>
+    <t>BALAGTAS, SHANEL DE GUZMAN</t>
+  </si>
+  <si>
+    <t>BALTAZAR, JULIEIANNA MARIE CRUZ</t>
+  </si>
+  <si>
+    <t>GRADE 8</t>
+  </si>
+  <si>
+    <t>CHASTITY:</t>
+  </si>
+  <si>
+    <t>Jerwin Soliman Cervantes</t>
+  </si>
+  <si>
+    <t>Gerald Mortalla Culala</t>
+  </si>
+  <si>
+    <t>Yesha Quiambao Camacho</t>
+  </si>
+  <si>
+    <t>Reynalyn Lucas Yambao</t>
+  </si>
+  <si>
+    <t>Jessa Yambao Sibug</t>
+  </si>
+  <si>
+    <t>COURAGE:</t>
+  </si>
+  <si>
+    <t>FAITH:</t>
+  </si>
+  <si>
+    <t>Ronald Alipaopao Cao</t>
+  </si>
+  <si>
+    <t>Jacob Mangulabnan Lapuz</t>
+  </si>
+  <si>
+    <t>Perly David Balidoy</t>
+  </si>
+  <si>
+    <t>Erika Chico Catalig</t>
+  </si>
+  <si>
+    <t>Nichole Magat Simbillo</t>
+  </si>
+  <si>
+    <t>HONOR:</t>
+  </si>
+  <si>
+    <t>CJ Tolentino Cao</t>
+  </si>
+  <si>
+    <t>Shered Sagum Chico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erich Pareña Butial </t>
+  </si>
+  <si>
+    <t>Kannery Carpio Larin</t>
+  </si>
+  <si>
+    <t>Chelssie Cruz Musni</t>
+  </si>
+  <si>
+    <t>HOPE:</t>
+  </si>
+  <si>
+    <t>Joseph Pangan Balingit</t>
+  </si>
+  <si>
+    <t>Kian Dela Cruz Frago</t>
+  </si>
+  <si>
+    <t>Jocel Larin Amante</t>
+  </si>
+  <si>
+    <t>Kate Caline Reyes Basa</t>
+  </si>
+  <si>
+    <t>Railyn Rondina Cariño</t>
+  </si>
+  <si>
+    <t>JUSTICE:</t>
+  </si>
+  <si>
+    <t>Kent Cabudol Estrada</t>
+  </si>
+  <si>
+    <t>Aldrin Dela Paz Talao</t>
+  </si>
+  <si>
+    <t>Elizabeth Talao Alfonso</t>
+  </si>
+  <si>
+    <t>Aleli Chico Manabat</t>
+  </si>
+  <si>
+    <t>Jessie Mempin Salas</t>
+  </si>
+  <si>
+    <t>HEMINGWAY:</t>
+  </si>
+  <si>
+    <t>ALCANTARA EARL ANGELO S.</t>
+  </si>
+  <si>
+    <t>DAVID, AEDHAN RALF</t>
+  </si>
+  <si>
+    <t>ARISTON, DENZIE FAYE M.</t>
+  </si>
+  <si>
+    <t>CASTRO M. JENICA</t>
+  </si>
+  <si>
+    <t>DE GUZMAN, AMIE ROSE T.</t>
+  </si>
+  <si>
+    <t>KILMER:</t>
+  </si>
+  <si>
+    <t>ANDAN, MARK JACOB</t>
+  </si>
+  <si>
+    <t>BALAJADIA, MC GAVIN</t>
+  </si>
+  <si>
+    <t>AGAS, APPLE</t>
+  </si>
+  <si>
+    <t>BAUTISTA, CRISTINE M.</t>
+  </si>
+  <si>
+    <t>BOLLUSA, MIA MARIEL P.</t>
+  </si>
+  <si>
+    <t>FROST:</t>
+  </si>
+  <si>
+    <t>ADARME, RAINIEL IMAS</t>
+  </si>
+  <si>
+    <t>ASI, CRISTIAN JAY LALU</t>
+  </si>
+  <si>
+    <t>CORNES, JANELLE DELA CRUZ</t>
+  </si>
+  <si>
+    <t>DELA PEÑA, LHIAN EUNICE VELADO.</t>
+  </si>
+  <si>
+    <t>MANALASTAS, ERICH LAPUZ</t>
+  </si>
+  <si>
+    <t>ORWELL:</t>
+  </si>
+  <si>
+    <t>CAVAN, RHOJET C.</t>
+  </si>
+  <si>
+    <t>DE LEON, JUSTIN B.</t>
+  </si>
+  <si>
+    <t>BARBOZA, JERICEL R</t>
+  </si>
+  <si>
+    <t>BARRIENTES, REALYNNE</t>
+  </si>
+  <si>
+    <t>HIPOLITO,MYCA</t>
+  </si>
+  <si>
+    <t>SHAKESPEARE:</t>
+  </si>
+  <si>
+    <t>AGUILA, JHON MEL. A</t>
+  </si>
+  <si>
+    <t>AGUILTO, JACK NOEL G.</t>
+  </si>
+  <si>
+    <t>AMANTE, JONALYN L.</t>
+  </si>
+  <si>
+    <t>BININI,KRIZETH FLORIE D.C</t>
+  </si>
+  <si>
+    <t>CASTRO,RHONA CRISELLE M.</t>
+  </si>
+  <si>
+    <t>TWAIN:</t>
+  </si>
+  <si>
+    <t>BACO, VHAL BEJERANO</t>
+  </si>
+  <si>
+    <t>BAYONGAN, JOHN MAR</t>
+  </si>
+  <si>
+    <t>CANTIGA, JILLIAN JHARICH</t>
+  </si>
+  <si>
+    <t>MANARANG, ROSEMARIE</t>
+  </si>
+  <si>
+    <t>PUNZALAN, JASMINE</t>
+  </si>
+  <si>
+    <t>ROWLING:</t>
+  </si>
+  <si>
+    <t>AMOR, JOHN REINNALD M.</t>
+  </si>
+  <si>
+    <t>CALEON, RANDY S.</t>
+  </si>
+  <si>
+    <t>BANTASAN, KARYL UNICE G.</t>
+  </si>
+  <si>
+    <t>BAUTISTA, MICA MAE G.</t>
+  </si>
+  <si>
+    <t>BERBA, LIE NIKKI</t>
+  </si>
+  <si>
+    <t>MORRISON:</t>
+  </si>
+  <si>
+    <t>CASTILLO, ANTHONY P.</t>
+  </si>
+  <si>
+    <t>DOMINGO, JOKO F.</t>
+  </si>
+  <si>
+    <t>AGUINALDO, MARIEL M.</t>
+  </si>
+  <si>
+    <t>CARPIO, QUENNIE A</t>
+  </si>
+  <si>
+    <t>DAVID, SOFIA V.</t>
+  </si>
+  <si>
+    <t>WHITMAN:</t>
+  </si>
+  <si>
+    <t>AQUINO, STEVEN F.</t>
+  </si>
+  <si>
+    <t>BANAAG, REYMARK R.</t>
+  </si>
+  <si>
+    <t>AGUINALDO, SHANE MARIAN</t>
+  </si>
+  <si>
+    <t>AMARO, ERRAH R.</t>
+  </si>
+  <si>
+    <t>BAGSIC, SHANE CHANEL B.</t>
+  </si>
+  <si>
+    <t>ANDERSEN:</t>
+  </si>
+  <si>
+    <t>BAYLON, ARVIE D.</t>
+  </si>
+  <si>
+    <t>BURAYOG, KHATE JOHN P.</t>
+  </si>
+  <si>
+    <t>ANDRES, SHANTAL B.</t>
+  </si>
+  <si>
+    <t>DE GUZMAN, STEPHANIE E.</t>
+  </si>
+  <si>
+    <t>INOCENCIO, PRINSSES LJ M.</t>
+  </si>
+  <si>
+    <t>GRADE 9</t>
   </si>
 </sst>
 </file>
@@ -260,7 +614,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -268,19 +622,471 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -563,61 +1369,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>3</v>
       </c>
     </row>
@@ -642,16 +1452,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -754,16 +1564,16 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -865,8 +1675,453 @@
         <v>55</v>
       </c>
     </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+    </row>
+    <row r="29" spans="1:6" s="16" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" spans="1:6" s="16" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="16" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="37"/>
+    </row>
+    <row r="38" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="J39" s="29" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J40" s="29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J41" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="J42" s="29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="G43" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H43" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="I43" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="J43" s="33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A37:J37"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="A11:C11"/>

</xml_diff>

<commit_message>
added all students and from
</commit_message>
<xml_diff>
--- a/dump/Students.xlsx
+++ b/dump/Students.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15075" windowHeight="7605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15075" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="Fulldata" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="367">
   <si>
     <t>Building 1</t>
   </si>
@@ -1132,7 +1131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1140,102 +1139,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="13">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="29">
@@ -1604,7 +1514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1693,200 +1603,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2170,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56:G60"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,26 +1929,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -2252,16 +1991,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2364,16 +2103,16 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83" t="s">
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2482,12 +2221,12 @@
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="87" t="s">
+      <c r="A21" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="88"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="89"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
@@ -2580,14 +2319,14 @@
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:6" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="90"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:6" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
@@ -2711,18 +2450,18 @@
     </row>
     <row r="36" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="84" t="s">
+      <c r="A37" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="B37" s="85"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="85"/>
-      <c r="J37" s="86"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
@@ -2918,17 +2657,17 @@
     </row>
     <row r="44" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="84" t="s">
+      <c r="A45" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="B45" s="85"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
       <c r="J45" s="31"/>
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
@@ -3153,17 +2892,17 @@
     </row>
     <row r="53" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="84" t="s">
+      <c r="A54" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="B54" s="85"/>
-      <c r="C54" s="85"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="85"/>
-      <c r="I54" s="86"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="34"/>
     </row>
     <row r="55" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
@@ -3341,19 +3080,19 @@
     </row>
     <row r="61" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="84" t="s">
+      <c r="A62" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="B62" s="85"/>
-      <c r="C62" s="85"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="85"/>
-      <c r="F62" s="85"/>
-      <c r="G62" s="85"/>
-      <c r="H62" s="85"/>
-      <c r="I62" s="85"/>
-      <c r="J62" s="85"/>
-      <c r="K62" s="86"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="34"/>
     </row>
     <row r="63" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
@@ -3568,12 +3307,6 @@
     <row r="69" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="A62:K62"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="A45:I45"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="A11:C11"/>
@@ -3581,771 +3314,12 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:I34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="89"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="42"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="43"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="44"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="44"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="44"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="45"/>
-    </row>
-    <row r="8" spans="1:6" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="90" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-    </row>
-    <row r="10" spans="1:6" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
-      <c r="B10" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" s="12" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="F11" s="56"/>
-    </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12" s="57"/>
-    </row>
-    <row r="13" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="58"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" s="57"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="59"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="84" t="s">
-        <v>188</v>
-      </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="85"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="86"/>
-    </row>
-    <row r="18" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="64"/>
-      <c r="H19" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J19" s="67"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="G20" s="64"/>
-      <c r="H20" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="J20" s="67"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="G21" s="64"/>
-      <c r="H21" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="J21" s="67"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="64"/>
-      <c r="H22" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="J22" s="67"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="G23" s="65"/>
-      <c r="H23" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="J23" s="68"/>
-    </row>
-    <row r="24" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="84" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-    </row>
-    <row r="26" spans="1:14" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="41"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-    </row>
-    <row r="27" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E27" s="69"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="66"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-    </row>
-    <row r="28" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="E28" s="69"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="66"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-    </row>
-    <row r="29" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="E29" s="69"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="66"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-    </row>
-    <row r="30" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30" s="69"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="66"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-    </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="E31" s="69"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="66"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-    </row>
-    <row r="33" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="84" t="s">
-        <v>299</v>
-      </c>
-      <c r="B34" s="85"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="86"/>
-    </row>
-    <row r="35" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>251</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>263</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="77"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="H36" s="79"/>
-      <c r="I36" s="95"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="H37" s="79"/>
-      <c r="I37" s="95"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="H38" s="79"/>
-      <c r="I38" s="95"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="H39" s="79"/>
-      <c r="I39" s="95"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="78"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="H40" s="80"/>
-      <c r="I40" s="96"/>
-    </row>
-    <row r="41" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="B42" s="85"/>
-      <c r="C42" s="85"/>
-      <c r="D42" s="85"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="85"/>
-      <c r="H42" s="85"/>
-      <c r="I42" s="85"/>
-      <c r="J42" s="85"/>
-      <c r="K42" s="86"/>
-    </row>
-    <row r="43" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>306</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>312</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>318</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>330</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="H43" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="I43" s="20" t="s">
-        <v>348</v>
-      </c>
-      <c r="J43" s="20" t="s">
-        <v>354</v>
-      </c>
-      <c r="K43" s="20" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="71"/>
-      <c r="B44" s="81"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="91"/>
-      <c r="K44" s="93"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="71"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="93"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="71"/>
-      <c r="B46" s="81"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="91"/>
-      <c r="K46" s="93"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="71"/>
-      <c r="B47" s="81"/>
-      <c r="C47" s="81"/>
-      <c r="D47" s="79"/>
-      <c r="E47" s="79"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="81"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="91"/>
-      <c r="K47" s="93"/>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="73"/>
-      <c r="B48" s="82"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="92"/>
-      <c r="K48" s="94"/>
-    </row>
-    <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="A62:K62"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A45:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>